<commit_message>
Add some extra file
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4381DE4-CA4A-4631-B500-B1DEA5343CB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DEAF07-0B91-4415-9324-ABC87528867A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7395" yWindow="2595" windowWidth="11940" windowHeight="9675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -580,7 +580,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>